<commit_message>
掲示板作成演習が完了！！# This is a combination of 2 commits.
[微修正]

コードレビューによる修正
</commit_message>
<xml_diff>
--- a/Document/掲示板テスト仕様書.xlsx
+++ b/Document/掲示板テスト仕様書.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="テスト仕様書" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="108">
   <si>
     <t>作成者</t>
     <rPh sb="0" eb="3">
@@ -1377,102 +1377,6 @@
     <t>INSERT INTO comments(name, content, article_id) VALUES('吉田2', '山田さん書き込みのコメント2',2);</t>
   </si>
   <si>
-    <t>「投稿者名：山田、投稿内容：新たな投稿です。」の掲示板の
-①名前に「testtesttesttesttesttesttesttesttesttesttesttesttest」（計５１文字）を入力する
-②コメントに「テストコメント」と入力する
-③コメント投稿ボタンをクリックする</t>
-    <rPh sb="1" eb="5">
-      <t>トウコウシャメイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ヤマダ</t>
-    </rPh>
-    <rPh sb="9" eb="13">
-      <t>トウコウナイヨウ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>アラ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>トウコウ</t>
-    </rPh>
-    <rPh sb="24" eb="27">
-      <t>ケイジバン</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>ケイ</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="95" eb="97">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="126" eb="128">
-      <t>トウコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・掲示板画面が表示されていること
-・「投稿者名：山田、投稿内容：新しい投稿です。」の掲示板の名前入力欄の上に「名前は49字以内で入力してください」という表示がされていること</t>
-    <rPh sb="1" eb="6">
-      <t>ケイジバンガメン</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="19" eb="23">
-      <t>トウコウシャメイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ヤマダ</t>
-    </rPh>
-    <rPh sb="27" eb="31">
-      <t>トウコウナイヨウ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>アタラ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>トウコウ</t>
-    </rPh>
-    <rPh sb="42" eb="45">
-      <t>ケイジバン</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>ラン</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="60" eb="63">
-      <t>ジイナイ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・掲示板画面が表示されていること
 ・「投稿者名：伊賀、投稿内容：この掲示板について」の掲示板の名前入力欄の上に「名前は50字以内で入力してください」という表示がされていること</t>
     <rPh sb="1" eb="6">
@@ -1913,12 +1817,282 @@
     <t>FOREIGN KEY (article_id) REFERENCES articles (id) ON DELETE CASCADE</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>大熊　隆寛</t>
+    <rPh sb="0" eb="2">
+      <t>オオクマ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>タカシ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ヒロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・掲示板画面が表示されていること
+・以下の掲示板が表示されていること
+-投稿者名：testtesttesttesttesttesttesttesttesttesttesttest12
+-投稿内容：テスト投稿</t>
+    <rPh sb="1" eb="6">
+      <t>ケイジバンガメン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>ケイジバン</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="36" eb="40">
+      <t>トウコウシャメイ</t>
+    </rPh>
+    <rPh sb="93" eb="97">
+      <t>トウコウナイヨウ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>トウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・掲示板画面が表示されていること
+・「投稿者名：山田、投稿内容：新しい投稿です。」の掲示板の名前入力欄の上に「名前は50字以内で入力してください」という表示がされていること</t>
+    <rPh sb="1" eb="6">
+      <t>ケイジバンガメン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="19" eb="23">
+      <t>トウコウシャメイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヤマダ</t>
+    </rPh>
+    <rPh sb="27" eb="31">
+      <t>トウコウナイヨウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="42" eb="45">
+      <t>ケイジバン</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="60" eb="63">
+      <t>ジイナイ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「投稿者名：山田、投稿内容：新たな投稿です。」の掲示板の
+①名前に「testtesttesttesttesttesttesttesttesttesttesttest12」（計５０文字）を入力する
+②コメントに「テストコメント」と入力する
+③コメント投稿ボタンをクリックする</t>
+    <rPh sb="1" eb="5">
+      <t>トウコウシャメイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ヤマダ</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>トウコウナイヨウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t>ケイジバン</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="86" eb="87">
+      <t>ケイ</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="124" eb="126">
+      <t>トウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「投稿者名：山田、投稿内容：新たな投稿です。」の掲示板の
+①名前に「testtesttesttesttesttesttesttesttesttesttesttest123」（計５１文字）を入力する
+②コメントに「テストコメント」と入力する
+③コメント投稿ボタンをクリックする</t>
+    <rPh sb="1" eb="5">
+      <t>トウコウシャメイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ヤマダ</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>トウコウナイヨウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t>ケイジバン</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>ケイ</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>トウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・掲示板画面が表示されていること
+・「投稿者名：伊賀、投稿内容：この掲示板について」の掲示板のコメントに以下の内容があること
+-コメント者名：testtesttesttesttesttesttesttesttesttesttesttest12
+-コメント内容：テストコメント</t>
+    <rPh sb="1" eb="6">
+      <t>ケイジバンガメン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="19" eb="23">
+      <t>トウコウシャメイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>イガ</t>
+    </rPh>
+    <rPh sb="27" eb="31">
+      <t>トウコウナイヨウ</t>
+    </rPh>
+    <rPh sb="34" eb="37">
+      <t>ケイジバン</t>
+    </rPh>
+    <rPh sb="43" eb="46">
+      <t>ケイジバン</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>シャメイ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>ナイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・掲示板画面が表示されていること
+・「投稿者名：山田、投稿内容：新しい投稿です。」の掲示板のコメントに以下の内容があること
+-コメント者名：testtesttesttesttesttesttesttesttesttesttesttest12
+-コメント内容：テストコメント</t>
+    <rPh sb="1" eb="6">
+      <t>ケイジバンガメン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="19" eb="23">
+      <t>トウコウシャメイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヤマダ</t>
+    </rPh>
+    <rPh sb="27" eb="31">
+      <t>トウコウナイヨウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="42" eb="45">
+      <t>ケイジバン</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>シャメイ</t>
+    </rPh>
+    <rPh sb="126" eb="128">
+      <t>ナイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1980,6 +2154,14 @@
       <color rgb="FF1D1C1D"/>
       <name val="Inherit"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2054,7 +2236,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2087,6 +2269,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2380,11 +2571,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.375" defaultRowHeight="13.5"/>
@@ -2395,22 +2586,22 @@
     <col min="4" max="4" width="34.125" style="4" customWidth="1"/>
     <col min="5" max="5" width="38.25" style="4" customWidth="1"/>
     <col min="6" max="6" width="46.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13.75" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="8" customWidth="1"/>
+    <col min="9" max="9" width="17.125" style="8" customWidth="1"/>
     <col min="10" max="16384" width="25.375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2419,13 +2610,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2480,11 +2671,17 @@
         <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="12">
+        <v>44344</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="121.5" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -2505,9 +2702,15 @@
       <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="G5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="12">
+        <v>44345</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="58.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -2528,9 +2731,15 @@
       <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="G6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="12">
+        <v>44346</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="84.75" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -2551,9 +2760,15 @@
       <c r="F7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="G7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="12">
+        <v>44347</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="87" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -2574,9 +2789,15 @@
       <c r="F8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="G8" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="12">
+        <v>44348</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:10" s="9" customFormat="1" ht="58.5" customHeight="1">
       <c r="A9" s="2" t="s">
@@ -2597,9 +2818,15 @@
       <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="G9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="12">
+        <v>44349</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:10" s="9" customFormat="1" ht="58.5" customHeight="1">
       <c r="A10" s="2" t="s">
@@ -2620,9 +2847,15 @@
       <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="G10" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="12">
+        <v>44350</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="9" customFormat="1" ht="114" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -2638,14 +2871,20 @@
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="12">
+        <v>44351</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="9" customFormat="1" ht="114" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -2661,14 +2900,20 @@
         <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="G12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="12">
+        <v>44352</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:10" s="9" customFormat="1" ht="137.25" customHeight="1">
       <c r="A13" s="2" t="s">
@@ -2689,9 +2934,15 @@
       <c r="F13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="G13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="12">
+        <v>44353</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="14" spans="1:10" s="9" customFormat="1" ht="66.75" customHeight="1">
       <c r="A14" s="2" t="s">
@@ -2712,9 +2963,15 @@
       <c r="F14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="G14" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="12">
+        <v>44354</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="15" spans="1:10" s="9" customFormat="1" ht="84.75" customHeight="1">
       <c r="A15" s="2" t="s">
@@ -2735,9 +2992,15 @@
       <c r="F15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="G15" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="12">
+        <v>44355</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" ht="117.75" customHeight="1">
       <c r="A16" s="2" t="s">
@@ -2758,9 +3021,15 @@
       <c r="F16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="G16" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="12">
+        <v>44356</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" ht="84.75" customHeight="1">
       <c r="A17" s="2" t="s">
@@ -2781,9 +3050,15 @@
       <c r="F17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="G17" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="12">
+        <v>44357</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" ht="84.75" customHeight="1">
       <c r="A18" s="2" t="s">
@@ -2804,11 +3079,17 @@
       <c r="F18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" ht="141.75" customHeight="1">
+      <c r="G18" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="12">
+        <v>44358</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="9" customFormat="1" ht="139.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -2822,16 +3103,22 @@
         <v>24</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" s="9" customFormat="1" ht="84.75" customHeight="1">
+        <v>107</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="12">
+        <v>44358</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="9" customFormat="1" ht="139.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -2839,20 +3126,26 @@
         <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="12">
+        <v>44359</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" ht="84.75" customHeight="1">
       <c r="A21" s="2" t="s">
@@ -2862,22 +3155,28 @@
         <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" ht="132.75" customHeight="1">
+        <v>89</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="12">
+        <v>44360</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="9" customFormat="1" ht="84.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -2885,22 +3184,28 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" ht="144.75" customHeight="1">
+        <v>91</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="12">
+        <v>44361</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="9" customFormat="1" ht="132.75" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2908,43 +3213,55 @@
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" ht="182.25" customHeight="1">
+        <v>106</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="12">
+        <v>44362</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="9" customFormat="1" ht="144.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="12">
+        <v>44363</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" ht="182.25" customHeight="1">
       <c r="A25" s="2" t="s">
@@ -2960,25 +3277,49 @@
         <v>50</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="12">
+        <v>44364</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="9" customFormat="1" ht="182.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" s="9" customFormat="1" ht="66.75" customHeight="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="F26" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H26" s="12">
+        <v>44365</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" ht="66.75" customHeight="1">
       <c r="A27" s="2"/>
@@ -2987,9 +3328,9 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" s="9" customFormat="1" ht="66.75" customHeight="1">
       <c r="A28" s="2"/>
@@ -2998,9 +3339,9 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" s="9" customFormat="1" ht="66.75" customHeight="1">
       <c r="A29" s="2"/>
@@ -3009,9 +3350,9 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" ht="66.75" customHeight="1">
       <c r="A30" s="2"/>
@@ -3020,9 +3361,9 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" ht="66.75" customHeight="1">
       <c r="A31" s="2"/>
@@ -3031,9 +3372,20 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" s="9" customFormat="1" ht="66.75" customHeight="1">
+      <c r="A32" s="2"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3049,7 +3401,7 @@
   <dimension ref="A1:A110"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3136,7 +3488,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -3446,7 +3798,7 @@
   <dimension ref="A1:A110"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3533,7 +3885,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -3828,8 +4180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3916,7 +4268,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:1">

</xml_diff>